<commit_message>
Modul Ajar Langkah Pembelajaran
</commit_message>
<xml_diff>
--- a/public/excel_template/Modul_Ajar_V2_Template.xlsx
+++ b/public/excel_template/Modul_Ajar_V2_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\API-Login-Register\public\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360F306-8EE6-44F4-B3DD-3C9F8F4AE2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44005447-F06B-4CA5-A1F5-80F2338E5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>MODUL AJAR</t>
   </si>
@@ -104,13 +104,25 @@
   </si>
   <si>
     <t>Daftar Pustaka</t>
+  </si>
+  <si>
+    <t>LANGKAH-LANGKAH PEMBELAJARAN</t>
+  </si>
+  <si>
+    <t>Kegiatan Awal</t>
+  </si>
+  <si>
+    <t>Kegiatan Inti</t>
+  </si>
+  <si>
+    <t>Kegiatan Penutup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,6 +181,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -224,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -254,10 +273,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,15 +499,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.85546875" customWidth="1"/>
     <col min="3" max="3" width="31.140625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
@@ -505,10 +528,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
@@ -613,10 +636,10 @@
       <c r="B22" s="6"/>
     </row>
     <row r="24" spans="1:2" ht="18.75">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="7" t="s">
@@ -667,37 +690,51 @@
       <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="B34" s="14"/>
-    </row>
-    <row r="35" spans="1:2" ht="18.75">
-      <c r="A35" s="15" t="s">
+      <c r="A34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A35" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A36" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A37" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1">
+      <c r="B38" s="14"/>
+    </row>
+    <row r="39" spans="1:2" ht="18.75">
+      <c r="A39" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="16"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="7" t="s">
+      <c r="B39" s="17"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="7" t="s">
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="B38" s="14"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="B39" s="14"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="B40" s="14"/>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="B41" s="14"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:2">
       <c r="B42" s="14"/>
@@ -710,13 +747,26 @@
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="14"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="14"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="14"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" s="14"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>